<commit_message>
Update PCB_Project_Mini mobile robot_2.xlsx
</commit_message>
<xml_diff>
--- a/Robot_Swarm_ShirazUni1399/PCB_Project_Mini mobile robot/Project Outputs for PCB_Project_Mini mobile robot/PCB_Project_Mini mobile robot_2.xlsx
+++ b/Robot_Swarm_ShirazUni1399/PCB_Project_Mini mobile robot/Project Outputs for PCB_Project_Mini mobile robot/PCB_Project_Mini mobile robot_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Mobile-Robot\Robot_Swarm_ShirazUni1399\PCB_Project_Mini mobile robot\Project Outputs for PCB_Project_Mini mobile robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BDBB60E-345D-453A-B8DF-EB96D28904A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E8BD2F-6D63-4B1A-8F68-6CD28E931F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="13455" xr2:uid="{F82E7417-9198-416B-A459-054874AE018A}"/>
+    <workbookView xWindow="690" yWindow="735" windowWidth="24645" windowHeight="13455" xr2:uid="{F82E7417-9198-416B-A459-054874AE018A}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_Project_Mini mobile robot_2" sheetId="1" r:id="rId1"/>
@@ -852,7 +852,9 @@
   </sheetPr>
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D56" sqref="A1:D56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1643,7 +1645,11 @@
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="35" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.30555555555555602" right="0.30555555555555602" top="0.60555555555555596" bottom="0.30555555555555602" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Bold"&amp;18Swarm Mobile Robot Project&amp;C&amp;"-,Bold"&amp;18ACRRL&amp;R&amp;"-,Bold"&amp;18Mohammad Sabouri</oddHeader>
+    <oddFooter>&amp;C&amp;P of 3</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>